<commit_message>
Eval reddit comments use case
</commit_message>
<xml_diff>
--- a/reddit-comments/reddit-comments-eval.xlsx
+++ b/reddit-comments/reddit-comments-eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ankushgarg/Desktop/MIDS/epic-data-lab/validate-LLM-graphs/reddit-comments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62AA6BE-EF7A-AA4E-A101-2DB628635649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF459640-98DD-D243-A57D-199169706A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="500" windowWidth="30240" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -865,7 +865,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>